<commit_message>
tried WordFilteringIndexingOptimizer and it didn't improve the results with the current words list
</commit_message>
<xml_diff>
--- a/improvements suggestions.xlsx
+++ b/improvements suggestions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NlpExercises\nlp-ex3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC1DFCF-7618-47EC-AD4D-7AA450FDF668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF715B6-FA60-4A9F-A230-47DD04A99899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Suggestion</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>MRR improved very slightly</t>
+  </si>
+  <si>
+    <t>worse results with current words list</t>
   </si>
 </sst>
 </file>
@@ -225,12 +228,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -245,12 +254,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,7 +548,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,7 +580,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D3">
@@ -593,7 +605,7 @@
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
@@ -618,6 +630,9 @@
       </c>
       <c r="D6">
         <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="55.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
removed hyde optimizer from final results - it is not deterministic and makes the recall, MRR values irrelevant
</commit_message>
<xml_diff>
--- a/improvements suggestions.xlsx
+++ b/improvements suggestions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NlpExercises\nlp-ex3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF715B6-FA60-4A9F-A230-47DD04A99899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CDCA1A-748F-4855-876C-A223E597153A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Suggestion</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>worse results with current words list</t>
+  </si>
+  <si>
+    <t>works well, improved results</t>
   </si>
 </sst>
 </file>
@@ -228,7 +231,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +241,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,6 +272,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -548,7 +560,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,7 +568,7 @@
     <col min="1" max="1" width="36.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.21875" style="2" customWidth="1"/>
     <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -622,7 +634,7 @@
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
@@ -635,12 +647,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -649,12 +661,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -668,7 +680,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -677,18 +689,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
marking the lemmatization as done
</commit_message>
<xml_diff>
--- a/improvements suggestions.xlsx
+++ b/improvements suggestions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NlpExercises\nlp-ex3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Aviv\nlp-ex3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CDCA1A-748F-4855-876C-A223E597153A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090C27CC-25CC-4012-9104-EB29ED101111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>Suggestion</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>works well, improved results</t>
+  </si>
+  <si>
+    <t>recall and mmr was signifactly imporved</t>
+  </si>
+  <si>
+    <t>used the dictaber after the trankit was not efficent</t>
   </si>
 </sst>
 </file>
@@ -213,7 +219,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -559,19 +565,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.19921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -591,7 +597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
@@ -599,21 +605,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -630,7 +639,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -647,7 +656,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -661,7 +670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -675,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -689,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -706,7 +715,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -720,7 +729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -734,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -748,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -762,7 +771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -776,7 +785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -790,7 +799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
small edit to improvements suggestions
</commit_message>
<xml_diff>
--- a/improvements suggestions.xlsx
+++ b/improvements suggestions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Aviv\nlp-ex3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NlpExercises\nlp-ex3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090C27CC-25CC-4012-9104-EB29ED101111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591DF9F7-0E52-4680-8848-9B63936DAAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>Suggestion</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>used the dictaber after the trankit was not efficent</t>
+  </si>
+  <si>
+    <t>it didn't work very well. Didn't find a tool that does a good job yet</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -565,19 +568,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.19921875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -597,7 +600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
@@ -605,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -622,7 +625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -635,11 +638,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -652,15 +655,15 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
@@ -669,8 +672,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -683,8 +689,9 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -697,8 +704,9 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -711,11 +719,11 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -728,8 +736,9 @@
       <c r="D11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -742,8 +751,9 @@
       <c r="D12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -756,8 +766,9 @@
       <c r="D13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="42" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -770,8 +781,9 @@
       <c r="D14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -784,8 +796,9 @@
       <c r="D15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -798,8 +811,9 @@
       <c r="D16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -812,6 +826,7 @@
       <c r="D17">
         <v>5</v>
       </c>
+      <c r="F17" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:F2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
added support for running rag on our dataset
</commit_message>
<xml_diff>
--- a/improvements suggestions.xlsx
+++ b/improvements suggestions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NlpExercises\nlp-ex3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591DF9F7-0E52-4680-8848-9B63936DAAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F765EE8-889E-4A75-AB82-AA8D5541D512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Suggestion</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>it didn't work very well. Didn't find a tool that does a good job yet</t>
+  </si>
+  <si>
+    <t>I tried it with AlephBert to find Synonm but it didn’t produce good words</t>
   </si>
 </sst>
 </file>
@@ -568,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,7 +683,7 @@
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
@@ -689,7 +692,9 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">

</xml_diff>